<commit_message>
update upload document ui
update upload document ui
</commit_message>
<xml_diff>
--- a/src/assets/doc/cashflow_detail_template.xlsx
+++ b/src/assets/doc/cashflow_detail_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peter\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{242576A2-4B1B-4E2B-852D-708C86957AB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{858908C8-8188-4513-99DB-9EB59D2E3BE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="49">
   <si>
     <t>Mục đích</t>
   </si>
@@ -39,12 +39,6 @@
     <t>Số lượng</t>
   </si>
   <si>
-    <t>Người trả</t>
-  </si>
-  <si>
-    <t>Người nhận</t>
-  </si>
-  <si>
     <t>STT</t>
   </si>
   <si>
@@ -127,6 +121,63 @@
   </si>
   <si>
     <t>Phần</t>
+  </si>
+  <si>
+    <t>END</t>
+  </si>
+  <si>
+    <t>Vui lòng không xóa dòng chữ "END" ở cuối bảng, đây là ký hiệu đánh dấu để chúng tôi biết dữ liệu trong bảng đã kết thúc</t>
+  </si>
+  <si>
+    <t>Tổng:</t>
+  </si>
+  <si>
+    <t>Địa chỉ</t>
+  </si>
+  <si>
+    <t>Người thanh toán</t>
+  </si>
+  <si>
+    <t>Đơn vị nhận</t>
+  </si>
+  <si>
+    <t>Học bổng mái ấm Ánh Sáng</t>
+  </si>
+  <si>
+    <t>Học bổng mái ấm Ga Sài Gòn</t>
+  </si>
+  <si>
+    <t>Học bổng mái ấm Hoa Mẫu Đơn</t>
+  </si>
+  <si>
+    <t>Học bổng mái ấm Truyền Tin</t>
+  </si>
+  <si>
+    <t>Mái ấm Ánh Sáng</t>
+  </si>
+  <si>
+    <t>Mái ấm Ga Sài Gòn</t>
+  </si>
+  <si>
+    <t>Mái ấm Hoa Mẫu Đơn</t>
+  </si>
+  <si>
+    <t>Mái ấm Truyền Tin</t>
+  </si>
+  <si>
+    <t>76 Trần Quang Diệu, Phường 14, Quận 3, Thành phố Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>739 Hoàng Sa, Phường 9, Quận 3, Thành phố Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>25 Đoàn Giỏi, Sơn Kỳ, Tân Phú, Thành phố Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>923/5 Tân Kỳ Tân Quý, Bình Hưng Hoà A, Bình Tân, Thành phố Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>Ông Trần Văn Dự</t>
   </si>
 </sst>
 </file>
@@ -135,8 +186,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="_([$VND]\ * #,##0_);_([$VND]\ * \(#,##0\);_([$VND]\ * &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="171" formatCode="[$-1010000]d/m/yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="_([$VND]\ * #,##0_);_([$VND]\ * \(#,##0\);_([$VND]\ * &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="[$-1010000]d/m/yyyy;@"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -177,7 +228,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -193,6 +244,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFBB800"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -247,7 +304,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -273,41 +330,50 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -336,13 +402,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>740003</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>295275</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>3619500</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>2390775</xdr:rowOff>
@@ -376,6 +442,61 @@
         <a:xfrm>
           <a:off x="9836378" y="923925"/>
           <a:ext cx="2879497" cy="2095500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>740003</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>3619500</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1828800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B4CDCDF7-1F3F-4B93-8696-7E8E3B99D22E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10318343" y="624840"/>
+          <a:ext cx="2879497" cy="1821180"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -709,86 +830,91 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B089CFBB-3DFB-405A-B3D9-041CB76827FA}">
-  <dimension ref="A1:J33"/>
+  <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
-    <col min="2" max="2" width="16.75" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.25" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.125" style="1" customWidth="1"/>
     <col min="4" max="4" width="10.25" style="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="1"/>
     <col min="6" max="6" width="16.625" style="10" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="57.25" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="9" style="1"/>
+    <col min="10" max="10" width="11.125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="57.25" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="18">
+    <row r="1" spans="1:11" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="23">
         <f>SUMPRODUCT(E:E, F:F)</f>
         <v>98200000</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-    </row>
-    <row r="2" spans="1:10" s="5" customFormat="1" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+    </row>
+    <row r="2" spans="1:11" s="5" customFormat="1" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" s="8" customFormat="1" ht="202.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="8" customFormat="1" ht="202.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15">
         <v>1</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E3" s="8">
         <v>1</v>
@@ -796,25 +922,25 @@
       <c r="F3" s="14">
         <v>1000000</v>
       </c>
-      <c r="G3" s="19" t="s">
-        <v>25</v>
+      <c r="G3" s="18" t="s">
+        <v>23</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15">
         <v>2</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E4" s="8">
         <v>4</v>
@@ -822,25 +948,25 @@
       <c r="F4" s="14">
         <v>1500000</v>
       </c>
-      <c r="G4" s="19" t="s">
-        <v>25</v>
+      <c r="G4" s="18" t="s">
+        <v>23</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15">
         <v>3</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E5" s="8">
         <v>12</v>
@@ -848,29 +974,30 @@
       <c r="F5" s="16">
         <v>1800000</v>
       </c>
-      <c r="G5" s="20" t="s">
+      <c r="G5" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H5" s="8" t="s">
-        <v>26</v>
-      </c>
       <c r="I5" s="17" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J5" s="17"/>
-    </row>
-    <row r="6" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K5" s="17"/>
+    </row>
+    <row r="6" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="15">
         <v>4</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E6" s="8">
         <v>10</v>
@@ -878,29 +1005,30 @@
       <c r="F6" s="16">
         <v>2000000</v>
       </c>
-      <c r="G6" s="20" t="s">
+      <c r="G6" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H6" s="8" t="s">
-        <v>26</v>
-      </c>
       <c r="I6" s="17" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J6" s="17"/>
-    </row>
-    <row r="7" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K6" s="17"/>
+    </row>
+    <row r="7" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="15">
         <v>5</v>
       </c>
       <c r="B7" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>17</v>
-      </c>
       <c r="D7" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E7" s="8">
         <v>14</v>
@@ -908,29 +1036,30 @@
       <c r="F7" s="16">
         <v>1500000</v>
       </c>
-      <c r="G7" s="20" t="s">
+      <c r="G7" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H7" s="8" t="s">
-        <v>26</v>
-      </c>
       <c r="I7" s="17" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J7" s="17"/>
-    </row>
-    <row r="8" spans="1:10" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K7" s="17"/>
+    </row>
+    <row r="8" spans="1:11" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="15">
         <v>6</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E8" s="8">
         <v>13</v>
@@ -938,62 +1067,72 @@
       <c r="F8" s="16">
         <v>2200000</v>
       </c>
-      <c r="G8" s="20" t="s">
+      <c r="G8" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H8" s="8" t="s">
-        <v>26</v>
-      </c>
       <c r="I8" s="17" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J8" s="17"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K8" s="17"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="20" t="s">
+        <v>30</v>
+      </c>
       <c r="F9" s="11"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K9" s="2"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F10" s="11"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K10" s="2"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F11" s="11"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K11" s="2"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F12" s="11"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K12" s="2"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F13" s="11"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K13" s="2"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F14" s="11"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
-    </row>
-    <row r="15" spans="1:10" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K14" s="2"/>
+    </row>
+    <row r="15" spans="1:11" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -1004,10 +1143,11 @@
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
       <c r="J15" s="6"/>
-    </row>
-    <row r="16" spans="1:10" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K15" s="6"/>
+    </row>
+    <row r="16" spans="1:11" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -1018,10 +1158,11 @@
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
       <c r="J16" s="6"/>
-    </row>
-    <row r="17" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K16" s="6"/>
+    </row>
+    <row r="17" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -1032,8 +1173,470 @@
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
       <c r="J17" s="6"/>
-    </row>
-    <row r="18" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K17" s="6"/>
+    </row>
+    <row r="18" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+    </row>
+    <row r="19" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+    </row>
+    <row r="20" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+    </row>
+    <row r="21" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+    </row>
+    <row r="22" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+    </row>
+    <row r="23" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F23" s="13"/>
+    </row>
+    <row r="24" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F24" s="13"/>
+    </row>
+    <row r="25" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F25" s="13"/>
+    </row>
+    <row r="26" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F26" s="13"/>
+    </row>
+    <row r="27" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F27" s="14"/>
+    </row>
+    <row r="28" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F28" s="14"/>
+    </row>
+    <row r="29" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F29" s="14"/>
+    </row>
+    <row r="30" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F30" s="14"/>
+    </row>
+    <row r="31" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F31" s="14"/>
+    </row>
+    <row r="32" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F32" s="14"/>
+    </row>
+    <row r="33" spans="6:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F33" s="14"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:K1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C91EB547-BA09-4826-8630-5CD42CD093CC}">
+  <dimension ref="A1:K26"/>
+  <sheetViews>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:K2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.625" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.875" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.75" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" style="8"/>
+    <col min="6" max="6" width="16.625" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.125" style="8" customWidth="1"/>
+    <col min="11" max="11" width="57.25" style="8" customWidth="1"/>
+    <col min="12" max="16384" width="9" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="21">
+        <f>SUMPRODUCT(E:E,F:F)</f>
+        <v>98200000</v>
+      </c>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+    </row>
+    <row r="2" spans="1:11" s="5" customFormat="1" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="147" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="15">
+        <v>1</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="8">
+        <v>1</v>
+      </c>
+      <c r="F3" s="8">
+        <v>1000000</v>
+      </c>
+      <c r="G3" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="15">
+        <v>2</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="8">
+        <v>4</v>
+      </c>
+      <c r="F4" s="8">
+        <v>1500000</v>
+      </c>
+      <c r="G4" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="15">
+        <v>3</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="8">
+        <v>12</v>
+      </c>
+      <c r="F5" s="17">
+        <v>1800000</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="I5" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="J5" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="K5" s="17"/>
+    </row>
+    <row r="6" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="15">
+        <v>4</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="8">
+        <v>10</v>
+      </c>
+      <c r="F6" s="17">
+        <v>2000000</v>
+      </c>
+      <c r="G6" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="I6" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="J6" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="K6" s="17"/>
+    </row>
+    <row r="7" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="15">
+        <v>5</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="8">
+        <v>14</v>
+      </c>
+      <c r="F7" s="17">
+        <v>1500000</v>
+      </c>
+      <c r="G7" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="I7" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="J7" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="K7" s="17"/>
+    </row>
+    <row r="8" spans="1:11" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A8" s="15">
+        <v>6</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="8">
+        <v>13</v>
+      </c>
+      <c r="F8" s="17">
+        <v>2200000</v>
+      </c>
+      <c r="G8" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="I8" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="J8" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="K8" s="17"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="16"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F10" s="16"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F11" s="16"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F12" s="16"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="17"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F13" s="16"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="17"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F14" s="16"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="17"/>
+    </row>
+    <row r="15" spans="1:11" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+    </row>
+    <row r="16" spans="1:11" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+    </row>
+    <row r="17" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+    </row>
+    <row r="18" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -1044,8 +1647,9 @@
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
       <c r="J18" s="6"/>
-    </row>
-    <row r="19" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K18" s="6"/>
+    </row>
+    <row r="19" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -1056,8 +1660,9 @@
       <c r="H19" s="6"/>
       <c r="I19" s="6"/>
       <c r="J19" s="6"/>
-    </row>
-    <row r="20" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K19" s="6"/>
+    </row>
+    <row r="20" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
@@ -1068,8 +1673,9 @@
       <c r="H20" s="6"/>
       <c r="I20" s="6"/>
       <c r="J20" s="6"/>
-    </row>
-    <row r="21" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K20" s="6"/>
+    </row>
+    <row r="21" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
@@ -1080,8 +1686,9 @@
       <c r="H21" s="6"/>
       <c r="I21" s="6"/>
       <c r="J21" s="6"/>
-    </row>
-    <row r="22" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K21" s="6"/>
+    </row>
+    <row r="22" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
@@ -1092,340 +1699,23 @@
       <c r="H22" s="6"/>
       <c r="I22" s="6"/>
       <c r="J22" s="6"/>
-    </row>
-    <row r="23" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K22" s="6"/>
+    </row>
+    <row r="23" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F23" s="13"/>
     </row>
-    <row r="24" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F24" s="13"/>
     </row>
-    <row r="25" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F25" s="13"/>
     </row>
-    <row r="26" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F26" s="13"/>
     </row>
-    <row r="27" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F27" s="14"/>
-    </row>
-    <row r="28" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F28" s="14"/>
-    </row>
-    <row r="29" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F29" s="14"/>
-    </row>
-    <row r="30" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F30" s="14"/>
-    </row>
-    <row r="31" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F31" s="14"/>
-    </row>
-    <row r="32" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F32" s="14"/>
-    </row>
-    <row r="33" spans="6:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F33" s="14"/>
-    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:J1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C91EB547-BA09-4826-8630-5CD42CD093CC}">
-  <dimension ref="A1:J33"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9" style="1"/>
-    <col min="2" max="2" width="16.75" style="1" customWidth="1"/>
-    <col min="3" max="3" width="29.125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="6.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9" style="1"/>
-    <col min="6" max="6" width="16.625" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="57.25" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="9" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="18">
-        <f>SUMPRODUCT(E:E, F:F)</f>
-        <v>0</v>
-      </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-    </row>
-    <row r="2" spans="1:10" s="5" customFormat="1" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" s="8" customFormat="1" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="15"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="19"/>
-    </row>
-    <row r="4" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="15"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="19"/>
-    </row>
-    <row r="5" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="20"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="17"/>
-    </row>
-    <row r="6" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="15"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="20"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
-    </row>
-    <row r="7" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="15"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="20"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17"/>
-    </row>
-    <row r="8" spans="1:10" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="15"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="20"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="17"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F9" s="11"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F10" s="11"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F11" s="11"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F12" s="11"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F13" s="11"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F14" s="11"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-    </row>
-    <row r="15" spans="1:10" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-    </row>
-    <row r="16" spans="1:10" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-    </row>
-    <row r="17" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
-    </row>
-    <row r="18" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
-    </row>
-    <row r="19" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-    </row>
-    <row r="20" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-    </row>
-    <row r="21" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-    </row>
-    <row r="22" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="6"/>
-    </row>
-    <row r="23" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F23" s="13"/>
-    </row>
-    <row r="24" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F24" s="13"/>
-    </row>
-    <row r="25" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F25" s="13"/>
-    </row>
-    <row r="26" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F26" s="13"/>
-    </row>
-    <row r="27" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F27" s="14"/>
-    </row>
-    <row r="28" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F28" s="14"/>
-    </row>
-    <row r="29" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F29" s="14"/>
-    </row>
-    <row r="30" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F30" s="14"/>
-    </row>
-    <row r="31" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F31" s="14"/>
-    </row>
-    <row r="32" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F32" s="14"/>
-    </row>
-    <row r="33" spans="6:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F33" s="14"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:J1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Fix navigate , login , org_detail
Fix navigate , login , org_detail
</commit_message>
<xml_diff>
--- a/src/assets/doc/cashflow_detail_template.xlsx
+++ b/src/assets/doc/cashflow_detail_template.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peter\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\Github\admin_web_v2\src\assets\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{858908C8-8188-4513-99DB-9EB59D2E3BE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="2" r:id="rId1"/>
     <sheet name="Cashflow" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="36">
   <si>
     <t>Mục đích</t>
   </si>
@@ -139,55 +138,16 @@
   </si>
   <si>
     <t>Đơn vị nhận</t>
-  </si>
-  <si>
-    <t>Học bổng mái ấm Ánh Sáng</t>
-  </si>
-  <si>
-    <t>Học bổng mái ấm Ga Sài Gòn</t>
-  </si>
-  <si>
-    <t>Học bổng mái ấm Hoa Mẫu Đơn</t>
-  </si>
-  <si>
-    <t>Học bổng mái ấm Truyền Tin</t>
-  </si>
-  <si>
-    <t>Mái ấm Ánh Sáng</t>
-  </si>
-  <si>
-    <t>Mái ấm Ga Sài Gòn</t>
-  </si>
-  <si>
-    <t>Mái ấm Hoa Mẫu Đơn</t>
-  </si>
-  <si>
-    <t>Mái ấm Truyền Tin</t>
-  </si>
-  <si>
-    <t>76 Trần Quang Diệu, Phường 14, Quận 3, Thành phố Hồ Chí Minh</t>
-  </si>
-  <si>
-    <t>739 Hoàng Sa, Phường 9, Quận 3, Thành phố Hồ Chí Minh</t>
-  </si>
-  <si>
-    <t>25 Đoàn Giỏi, Sơn Kỳ, Tân Phú, Thành phố Hồ Chí Minh</t>
-  </si>
-  <si>
-    <t>923/5 Tân Kỳ Tân Quý, Bình Hưng Hoà A, Bình Tân, Thành phố Hồ Chí Minh</t>
-  </si>
-  <si>
-    <t>Ông Trần Văn Dự</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_([$VND]\ * #,##0_);_([$VND]\ * \(#,##0\);_([$VND]\ * &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="[$-1010000]d/m/yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_([$VND]\ * #,##0_);_([$VND]\ * \(#,##0\);_([$VND]\ * &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="[$-1010000]d/m/yyyy;@"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -302,7 +262,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -330,37 +290,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -372,7 +332,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -442,61 +402,6 @@
         <a:xfrm>
           <a:off x="9836378" y="923925"/>
           <a:ext cx="2879497" cy="2095500"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>740003</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>3619500</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>1828800</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B4CDCDF7-1F3F-4B93-8696-7E8E3B99D22E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="10318343" y="624840"/>
-          <a:ext cx="2879497" cy="1821180"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -829,30 +734,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B089CFBB-3DFB-405A-B3D9-041CB76827FA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
-    <col min="2" max="2" width="17.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.25" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.09765625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.19921875" style="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="1"/>
-    <col min="6" max="6" width="16.625" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.59765625" style="10" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.5" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="57.25" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.09765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.09765625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="57.19921875" style="1" customWidth="1"/>
     <col min="12" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:11" ht="31.8" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A1" s="23">
         <f>SUMPRODUCT(E:E, F:F)</f>
         <v>98200000</v>
@@ -868,7 +773,7 @@
       <c r="J1" s="23"/>
       <c r="K1" s="23"/>
     </row>
-    <row r="2" spans="1:11" s="5" customFormat="1" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" s="5" customFormat="1" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -903,7 +808,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="8" customFormat="1" ht="202.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" s="8" customFormat="1" ht="202.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15">
         <v>1</v>
       </c>
@@ -929,7 +834,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" s="8" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A4" s="15">
         <v>2</v>
       </c>
@@ -955,7 +860,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" s="8" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A5" s="15">
         <v>3</v>
       </c>
@@ -986,7 +891,7 @@
       <c r="J5" s="17"/>
       <c r="K5" s="17"/>
     </row>
-    <row r="6" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="15">
         <v>4</v>
       </c>
@@ -1017,7 +922,7 @@
       <c r="J6" s="17"/>
       <c r="K6" s="17"/>
     </row>
-    <row r="7" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="15">
         <v>5</v>
       </c>
@@ -1048,7 +953,7 @@
       <c r="J7" s="17"/>
       <c r="K7" s="17"/>
     </row>
-    <row r="8" spans="1:11" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="15">
         <v>6</v>
       </c>
@@ -1079,7 +984,7 @@
       <c r="J8" s="17"/>
       <c r="K8" s="17"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
         <v>30</v>
       </c>
@@ -1090,7 +995,7 @@
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="F10" s="11"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
@@ -1098,7 +1003,7 @@
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="F11" s="11"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
@@ -1106,7 +1011,7 @@
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="F12" s="11"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
@@ -1114,7 +1019,7 @@
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="F13" s="11"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
@@ -1122,7 +1027,7 @@
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="F14" s="11"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
@@ -1130,7 +1035,7 @@
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="1:11" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>17</v>
       </c>
@@ -1145,7 +1050,7 @@
       <c r="J15" s="6"/>
       <c r="K15" s="6"/>
     </row>
-    <row r="16" spans="1:11" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>5</v>
       </c>
@@ -1160,7 +1065,7 @@
       <c r="J16" s="6"/>
       <c r="K16" s="6"/>
     </row>
-    <row r="17" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
         <v>16</v>
       </c>
@@ -1175,7 +1080,7 @@
       <c r="J17" s="6"/>
       <c r="K17" s="6"/>
     </row>
-    <row r="18" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>31</v>
       </c>
@@ -1190,7 +1095,7 @@
       <c r="J18" s="6"/>
       <c r="K18" s="6"/>
     </row>
-    <row r="19" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -1203,7 +1108,7 @@
       <c r="J19" s="6"/>
       <c r="K19" s="6"/>
     </row>
-    <row r="20" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
@@ -1216,7 +1121,7 @@
       <c r="J20" s="6"/>
       <c r="K20" s="6"/>
     </row>
-    <row r="21" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
@@ -1229,7 +1134,7 @@
       <c r="J21" s="6"/>
       <c r="K21" s="6"/>
     </row>
-    <row r="22" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="6"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
@@ -1242,37 +1147,37 @@
       <c r="J22" s="6"/>
       <c r="K22" s="6"/>
     </row>
-    <row r="23" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F23" s="13"/>
     </row>
-    <row r="24" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F24" s="13"/>
     </row>
-    <row r="25" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F25" s="13"/>
     </row>
-    <row r="26" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F26" s="13"/>
     </row>
-    <row r="27" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F27" s="14"/>
     </row>
-    <row r="28" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F28" s="14"/>
     </row>
-    <row r="29" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F29" s="14"/>
     </row>
-    <row r="30" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F30" s="14"/>
     </row>
-    <row r="31" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F31" s="14"/>
     </row>
-    <row r="32" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F32" s="14"/>
     </row>
-    <row r="33" spans="6:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="6:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F33" s="14"/>
     </row>
   </sheetData>
@@ -1286,36 +1191,36 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C91EB547-BA09-4826-8630-5CD42CD093CC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:K2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.625" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.875" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.75" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.59765625" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.8984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.69921875" style="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.5" style="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="8"/>
-    <col min="6" max="6" width="16.625" style="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.59765625" style="14" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.5" style="8" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.5" style="8" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19.5" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.125" style="8" customWidth="1"/>
-    <col min="11" max="11" width="57.25" style="8" customWidth="1"/>
+    <col min="10" max="10" width="11.09765625" style="8" customWidth="1"/>
+    <col min="11" max="11" width="57.19921875" style="8" customWidth="1"/>
     <col min="12" max="16384" width="9" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="21" t="s">
         <v>32</v>
       </c>
       <c r="B1" s="21">
         <f>SUMPRODUCT(E:E,F:F)</f>
-        <v>98200000</v>
+        <v>0</v>
       </c>
       <c r="C1" s="21"/>
       <c r="D1" s="21"/>
@@ -1327,7 +1232,7 @@
       <c r="J1" s="21"/>
       <c r="K1" s="21"/>
     </row>
-    <row r="2" spans="1:11" s="5" customFormat="1" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" s="5" customFormat="1" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -1362,191 +1267,49 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="147" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="15">
-        <v>1</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" s="8">
-        <v>1</v>
-      </c>
-      <c r="F3" s="8">
-        <v>1000000</v>
-      </c>
-      <c r="G3" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="15">
-        <v>2</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" s="8">
-        <v>4</v>
-      </c>
-      <c r="F4" s="8">
-        <v>1500000</v>
-      </c>
-      <c r="G4" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="15">
-        <v>3</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" s="8">
-        <v>12</v>
-      </c>
-      <c r="F5" s="17">
-        <v>1800000</v>
-      </c>
-      <c r="G5" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="I5" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="J5" s="17" t="s">
-        <v>44</v>
-      </c>
+    <row r="3" spans="1:11" ht="147" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="15"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="18"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="15"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="18"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="15"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="19"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
       <c r="K5" s="17"/>
     </row>
-    <row r="6" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="15">
-        <v>4</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" s="8">
-        <v>10</v>
-      </c>
-      <c r="F6" s="17">
-        <v>2000000</v>
-      </c>
-      <c r="G6" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="I6" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="J6" s="17" t="s">
-        <v>45</v>
-      </c>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="15"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="19"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
       <c r="K6" s="17"/>
     </row>
-    <row r="7" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="15">
-        <v>5</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" s="8">
-        <v>14</v>
-      </c>
-      <c r="F7" s="17">
-        <v>1500000</v>
-      </c>
-      <c r="G7" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="I7" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="J7" s="17" t="s">
-        <v>46</v>
-      </c>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="15"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="19"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
       <c r="K7" s="17"/>
     </row>
-    <row r="8" spans="1:11" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A8" s="15">
-        <v>6</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" s="8">
-        <v>13</v>
-      </c>
-      <c r="F8" s="17">
-        <v>2200000</v>
-      </c>
-      <c r="G8" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="I8" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="J8" s="17" t="s">
-        <v>47</v>
-      </c>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="15"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="19"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
       <c r="K8" s="17"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="22" t="s">
         <v>30</v>
       </c>
@@ -1557,7 +1320,7 @@
       <c r="J9" s="17"/>
       <c r="K9" s="17"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="F10" s="16"/>
       <c r="G10" s="17"/>
       <c r="H10" s="17"/>
@@ -1565,7 +1328,7 @@
       <c r="J10" s="17"/>
       <c r="K10" s="17"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="F11" s="16"/>
       <c r="G11" s="17"/>
       <c r="H11" s="17"/>
@@ -1573,7 +1336,7 @@
       <c r="J11" s="17"/>
       <c r="K11" s="17"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="F12" s="16"/>
       <c r="G12" s="17"/>
       <c r="H12" s="17"/>
@@ -1581,7 +1344,7 @@
       <c r="J12" s="17"/>
       <c r="K12" s="17"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="F13" s="16"/>
       <c r="G13" s="17"/>
       <c r="H13" s="17"/>
@@ -1589,7 +1352,7 @@
       <c r="J13" s="17"/>
       <c r="K13" s="17"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="F14" s="16"/>
       <c r="G14" s="17"/>
       <c r="H14" s="17"/>
@@ -1597,7 +1360,7 @@
       <c r="J14" s="17"/>
       <c r="K14" s="17"/>
     </row>
-    <row r="15" spans="1:11" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -1610,7 +1373,7 @@
       <c r="J15" s="6"/>
       <c r="K15" s="6"/>
     </row>
-    <row r="16" spans="1:11" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -1623,7 +1386,7 @@
       <c r="J16" s="6"/>
       <c r="K16" s="6"/>
     </row>
-    <row r="17" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -1636,7 +1399,7 @@
       <c r="J17" s="6"/>
       <c r="K17" s="6"/>
     </row>
-    <row r="18" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -1649,7 +1412,7 @@
       <c r="J18" s="6"/>
       <c r="K18" s="6"/>
     </row>
-    <row r="19" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -1662,7 +1425,7 @@
       <c r="J19" s="6"/>
       <c r="K19" s="6"/>
     </row>
-    <row r="20" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
@@ -1675,7 +1438,7 @@
       <c r="J20" s="6"/>
       <c r="K20" s="6"/>
     </row>
-    <row r="21" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
@@ -1688,7 +1451,7 @@
       <c r="J21" s="6"/>
       <c r="K21" s="6"/>
     </row>
-    <row r="22" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="6"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
@@ -1701,21 +1464,20 @@
       <c r="J22" s="6"/>
       <c r="K22" s="6"/>
     </row>
-    <row r="23" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F23" s="13"/>
     </row>
-    <row r="24" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F24" s="13"/>
     </row>
-    <row r="25" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F25" s="13"/>
     </row>
-    <row r="26" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F26" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>